<commit_message>
alternate approach to prism C
</commit_message>
<xml_diff>
--- a/MCNP/wedge_data_2025-12-31.xlsx
+++ b/MCNP/wedge_data_2025-12-31.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\MCNP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB8640-83BF-45A8-9CDD-E31A01C958C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5854B0-AF63-4BB8-8857-9D67A8A7182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28824" yWindow="2376" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FC2A7-2007-48F8-8A3D-08B47124466B}">
   <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2315,7 +2315,7 @@
         <v>42</v>
       </c>
       <c r="J44" s="2">
-        <v>1.7915200000000001E-5</v>
+        <v>2.0225799999999999E-5</v>
       </c>
       <c r="K44" s="30">
         <f t="shared" ref="K44:K52" si="11">P44*$T$4*$W$3*1E-24</f>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="M44" s="11">
         <f>J44/H44</f>
-        <v>0.50790745905844814</v>
+        <v>0.57341445730018981</v>
       </c>
       <c r="N44" s="11">
         <f t="shared" ref="N44:N56" si="12">K44/H44</f>
@@ -2365,7 +2365,7 @@
         <v>43</v>
       </c>
       <c r="J45" s="5">
-        <v>9.4329300000000005E-5</v>
+        <v>1.07538E-4</v>
       </c>
       <c r="K45" s="31">
         <f t="shared" si="11"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="M45" s="9">
         <f t="shared" ref="M45:M56" si="14">J45/H45</f>
-        <v>0.53569327578727111</v>
+        <v>0.610705088361851</v>
       </c>
       <c r="N45" s="9">
         <f t="shared" si="12"/>
@@ -2464,7 +2464,9 @@
       <c r="I47" s="21">
         <v>2.8804099999999999E-3</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="J47" s="5">
+        <v>3.2061199999999998E-3</v>
+      </c>
       <c r="K47" s="31">
         <f t="shared" si="11"/>
         <v>2.5144030799999998E-3</v>
@@ -2475,7 +2477,7 @@
       </c>
       <c r="M47" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.63798829264279977</v>
       </c>
       <c r="N47" s="9">
         <f t="shared" si="12"/>
@@ -2512,7 +2514,9 @@
       <c r="I48" s="16">
         <v>5.7066199999999999E-3</v>
       </c>
-      <c r="J48" s="2"/>
+      <c r="J48" s="2">
+        <v>6.3816400000000001E-3</v>
+      </c>
       <c r="K48" s="30">
         <f t="shared" si="11"/>
         <v>5.1434879999999999E-3</v>
@@ -2523,7 +2527,7 @@
       </c>
       <c r="M48" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.66408470901069316</v>
       </c>
       <c r="N48" s="11">
         <f t="shared" si="12"/>
@@ -2560,7 +2564,9 @@
       <c r="I49" s="17">
         <v>1.13375E-2</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49" s="5">
+        <v>1.26023E-2</v>
+      </c>
       <c r="K49" s="31">
         <f t="shared" si="11"/>
         <v>1.25591816E-2</v>
@@ -2571,7 +2577,7 @@
       </c>
       <c r="M49" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.70183546417238152</v>
       </c>
       <c r="N49" s="9">
         <f t="shared" si="12"/>
@@ -2608,7 +2614,9 @@
       <c r="I50" s="16">
         <v>1.6732899999999998E-2</v>
       </c>
-      <c r="J50" s="2"/>
+      <c r="J50" s="2">
+        <v>1.8516899999999999E-2</v>
+      </c>
       <c r="K50" s="30">
         <f t="shared" si="11"/>
         <v>1.8564839299999997E-2</v>
@@ -2619,7 +2627,7 @@
       </c>
       <c r="M50" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.72696064437422026</v>
       </c>
       <c r="N50" s="11">
         <f t="shared" si="12"/>
@@ -2656,7 +2664,9 @@
       <c r="I51" s="17">
         <v>2.1914300000000001E-2</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="J51" s="5">
+        <v>2.44475E-2</v>
+      </c>
       <c r="K51" s="31">
         <f t="shared" si="11"/>
         <v>2.4434994500000001E-2</v>
@@ -2667,7 +2677,7 @@
       </c>
       <c r="M51" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.75414181471346997</v>
       </c>
       <c r="N51" s="9">
         <f t="shared" si="12"/>
@@ -2704,7 +2714,9 @@
       <c r="I52" s="16">
         <v>2.7247799999999999E-2</v>
       </c>
-      <c r="J52" s="2"/>
+      <c r="J52" s="2">
+        <v>3.0182199999999999E-2</v>
+      </c>
       <c r="K52" s="30">
         <f t="shared" si="11"/>
         <v>3.0129525999999997E-2</v>
@@ -2715,7 +2727,7 @@
       </c>
       <c r="M52" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.77280848853880657</v>
       </c>
       <c r="N52" s="11">
         <f t="shared" si="12"/>

</xml_diff>

<commit_message>
wedge model adjusts done
</commit_message>
<xml_diff>
--- a/MCNP/wedge_data_2025-12-31.xlsx
+++ b/MCNP/wedge_data_2025-12-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\MCNP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5854B0-AF63-4BB8-8857-9D67A8A7182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78376352-570C-4FAC-9F27-6FF993714211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>BISO vol%</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Homog.</t>
-  </si>
-  <si>
-    <t>MCNP DATA COLLATED</t>
   </si>
 </sst>
 </file>
@@ -332,9 +329,9 @@
     <xf numFmtId="11" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FC2A7-2007-48F8-8A3D-08B47124466B}">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,15 +1586,15 @@
         <f>P27*$T$4*$W$3*1E-24</f>
         <v>2.0764465399999998E-5</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="31">
         <f t="shared" ref="L27:L39" si="6">I27/H27</f>
         <v>0.62980105333714986</v>
       </c>
-      <c r="M27" s="29">
+      <c r="M27" s="31">
         <f t="shared" ref="M27:M39" si="7">J27/H27</f>
         <v>0.63813897776495931</v>
       </c>
-      <c r="N27" s="29">
+      <c r="N27" s="31">
         <f t="shared" ref="N27:N39" si="8">K27/H27</f>
         <v>0.58868596834090958</v>
       </c>
@@ -1638,15 +1635,15 @@
         <f t="shared" ref="K28:K39" si="9">P28*$T$4*$W$3*1E-24</f>
         <v>1.1061240399999999E-4</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="9">
         <f t="shared" si="6"/>
         <v>0.60327131647967303</v>
       </c>
-      <c r="M28" s="29">
+      <c r="M28" s="9">
         <f t="shared" si="7"/>
         <v>0.57044119023760176</v>
       </c>
-      <c r="N28" s="29">
+      <c r="N28" s="9">
         <f t="shared" si="8"/>
         <v>0.62816453680314643</v>
       </c>
@@ -2131,15 +2128,15 @@
         <f t="shared" si="9"/>
         <v>0.12434955399999999</v>
       </c>
-      <c r="L38" s="29">
+      <c r="L38" s="9">
         <f t="shared" si="6"/>
         <v>0.91905084046829388</v>
       </c>
-      <c r="M38" s="29">
+      <c r="M38" s="9">
         <f t="shared" si="7"/>
         <v>0.86056372078801013</v>
       </c>
-      <c r="N38" s="29">
+      <c r="N38" s="9">
         <f t="shared" si="8"/>
         <v>0.85643514448750746</v>
       </c>
@@ -2180,15 +2177,15 @@
         <f t="shared" si="9"/>
         <v>0.16219431200000001</v>
       </c>
-      <c r="L39" s="29">
+      <c r="L39" s="31">
         <f t="shared" si="6"/>
         <v>0.94246398594536107</v>
       </c>
-      <c r="M39" s="29">
+      <c r="M39" s="31">
         <f t="shared" si="7"/>
         <v>0.85681966957018219</v>
       </c>
-      <c r="N39" s="29">
+      <c r="N39" s="31">
         <f t="shared" si="8"/>
         <v>0.87238717397365373</v>
       </c>
@@ -2315,9 +2312,9 @@
         <v>42</v>
       </c>
       <c r="J44" s="2">
-        <v>2.0225799999999999E-5</v>
-      </c>
-      <c r="K44" s="30">
+        <v>2.1465299999999999E-5</v>
+      </c>
+      <c r="K44" s="29">
         <f t="shared" ref="K44:K52" si="11">P44*$T$4*$W$3*1E-24</f>
         <v>2.0412221199999998E-5</v>
       </c>
@@ -2327,14 +2324,14 @@
       </c>
       <c r="M44" s="11">
         <f>J44/H44</f>
-        <v>0.57341445730018981</v>
+        <v>0.60855508065370789</v>
       </c>
       <c r="N44" s="11">
         <f t="shared" ref="N44:N56" si="12">K44/H44</f>
         <v>0.57869961839281658</v>
       </c>
       <c r="O44" s="4"/>
-      <c r="P44" s="30">
+      <c r="P44" s="29">
         <v>3.27644</v>
       </c>
       <c r="Q44" s="2"/>
@@ -2367,7 +2364,7 @@
       <c r="J45" s="5">
         <v>1.07538E-4</v>
       </c>
-      <c r="K45" s="31">
+      <c r="K45" s="30">
         <f t="shared" si="11"/>
         <v>1.0768492699999999E-4</v>
       </c>
@@ -2384,7 +2381,7 @@
         <v>0.61153948240412204</v>
       </c>
       <c r="O45" s="4"/>
-      <c r="P45" s="31">
+      <c r="P45" s="30">
         <v>17.2849</v>
       </c>
       <c r="Q45" s="5"/>
@@ -2417,7 +2414,7 @@
       <c r="J46" s="2">
         <v>2.9638700000000001E-4</v>
       </c>
-      <c r="K46" s="30">
+      <c r="K46" s="29">
         <f t="shared" si="11"/>
         <v>2.97874367E-4</v>
       </c>
@@ -2434,7 +2431,7 @@
         <v>0.56539039627950438</v>
       </c>
       <c r="O46" s="4"/>
-      <c r="P46" s="30">
+      <c r="P46" s="29">
         <v>47.812899999999999</v>
       </c>
       <c r="Q46" s="2"/>
@@ -2467,7 +2464,7 @@
       <c r="J47" s="5">
         <v>3.2061199999999998E-3</v>
       </c>
-      <c r="K47" s="31">
+      <c r="K47" s="30">
         <f t="shared" si="11"/>
         <v>2.5144030799999998E-3</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>0.50034300900309314</v>
       </c>
       <c r="O47" s="4"/>
-      <c r="P47" s="31">
+      <c r="P47" s="30">
         <v>403.596</v>
       </c>
       <c r="Q47" s="5"/>
@@ -2517,7 +2514,7 @@
       <c r="J48" s="2">
         <v>6.3816400000000001E-3</v>
       </c>
-      <c r="K48" s="30">
+      <c r="K48" s="29">
         <f t="shared" si="11"/>
         <v>5.1434879999999999E-3</v>
       </c>
@@ -2534,7 +2531,7 @@
         <v>0.53524042907152269</v>
       </c>
       <c r="O48" s="4"/>
-      <c r="P48" s="30">
+      <c r="P48" s="29">
         <v>825.6</v>
       </c>
       <c r="Q48" s="2"/>
@@ -2567,7 +2564,7 @@
       <c r="J49" s="5">
         <v>1.26023E-2</v>
       </c>
-      <c r="K49" s="31">
+      <c r="K49" s="30">
         <f t="shared" si="11"/>
         <v>1.25591816E-2</v>
       </c>
@@ -2584,7 +2581,7 @@
         <v>0.69943415470677839</v>
       </c>
       <c r="O49" s="4"/>
-      <c r="P49" s="31">
+      <c r="P49" s="30">
         <v>2015.92</v>
       </c>
       <c r="Q49" s="5"/>
@@ -2617,7 +2614,7 @@
       <c r="J50" s="2">
         <v>1.8516899999999999E-2</v>
       </c>
-      <c r="K50" s="30">
+      <c r="K50" s="29">
         <f t="shared" si="11"/>
         <v>1.8564839299999997E-2</v>
       </c>
@@ -2634,7 +2631,7 @@
         <v>0.72884270802520112</v>
       </c>
       <c r="O50" s="4"/>
-      <c r="P50" s="30">
+      <c r="P50" s="29">
         <v>2979.91</v>
       </c>
       <c r="Q50" s="2"/>
@@ -2667,7 +2664,7 @@
       <c r="J51" s="5">
         <v>2.44475E-2</v>
       </c>
-      <c r="K51" s="31">
+      <c r="K51" s="30">
         <f t="shared" si="11"/>
         <v>2.4434994500000001E-2</v>
       </c>
@@ -2684,7 +2681,7 @@
         <v>0.75375605255112621</v>
       </c>
       <c r="O51" s="4"/>
-      <c r="P51" s="31">
+      <c r="P51" s="30">
         <v>3922.15</v>
       </c>
       <c r="Q51" s="5"/>
@@ -2717,7 +2714,7 @@
       <c r="J52" s="2">
         <v>3.0182199999999999E-2</v>
       </c>
-      <c r="K52" s="30">
+      <c r="K52" s="29">
         <f t="shared" si="11"/>
         <v>3.0129525999999997E-2</v>
       </c>
@@ -2734,7 +2731,7 @@
         <v>0.77145978253575531</v>
       </c>
       <c r="O52" s="4"/>
-      <c r="P52" s="30">
+      <c r="P52" s="29">
         <v>4836.2</v>
       </c>
       <c r="Q52" s="2"/>
@@ -2764,8 +2761,10 @@
       <c r="I53" s="17">
         <v>4.3543999999999999E-2</v>
       </c>
-      <c r="J53" s="5"/>
-      <c r="K53" s="31">
+      <c r="J53" s="5">
+        <v>4.8447299999999999E-2</v>
+      </c>
+      <c r="K53" s="30">
         <f>P53*$T$5*$W$3*1E-24+0.008</f>
         <v>4.7207570499999997E-2</v>
       </c>
@@ -2775,14 +2774,14 @@
       </c>
       <c r="M53" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.82137283592286769</v>
       </c>
       <c r="N53" s="9">
         <f t="shared" si="12"/>
         <v>0.80035453077083152</v>
       </c>
       <c r="O53" s="4"/>
-      <c r="P53" s="31">
+      <c r="P53" s="30">
         <v>6293.35</v>
       </c>
       <c r="Q53" s="5"/>
@@ -2812,8 +2811,10 @@
       <c r="I54" s="16">
         <v>8.01066E-2</v>
       </c>
-      <c r="J54" s="2"/>
-      <c r="K54" s="30">
+      <c r="J54" s="2">
+        <v>8.9392399999999997E-2</v>
+      </c>
+      <c r="K54" s="29">
         <f>P54*$T$4*$W$3*1E-24</f>
         <v>8.9221698999999988E-2</v>
       </c>
@@ -2823,14 +2824,14 @@
       </c>
       <c r="M54" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.86290194261690956</v>
       </c>
       <c r="N54" s="11">
         <f t="shared" si="12"/>
         <v>0.86125417139131699</v>
       </c>
       <c r="O54" s="4"/>
-      <c r="P54" s="30">
+      <c r="P54" s="29">
         <v>14321.3</v>
       </c>
       <c r="Q54" s="2"/>
@@ -2860,8 +2861,10 @@
       <c r="I55" s="17">
         <v>0.114644</v>
       </c>
-      <c r="J55" s="5"/>
-      <c r="K55" s="31">
+      <c r="J55" s="5">
+        <v>0.12684899999999999</v>
+      </c>
+      <c r="K55" s="30">
         <f>P55*$T$4*$W$3*1E-24</f>
         <v>0.126647801</v>
       </c>
@@ -2871,14 +2874,14 @@
       </c>
       <c r="M55" s="9">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.87364962839429117</v>
       </c>
       <c r="N55" s="9">
         <f t="shared" si="12"/>
         <v>0.87226390653930375</v>
       </c>
       <c r="O55" s="4"/>
-      <c r="P55" s="31">
+      <c r="P55" s="30">
         <v>20328.7</v>
       </c>
       <c r="Q55" s="5"/>
@@ -2906,8 +2909,10 @@
         <v>0.185920101577397</v>
       </c>
       <c r="I56" s="16"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="30">
+      <c r="J56" s="2">
+        <v>0.162772</v>
+      </c>
+      <c r="K56" s="29">
         <f>P56*$T$4*$W$3*1E-24</f>
         <v>0.16153143999999997</v>
       </c>
@@ -2917,703 +2922,16 @@
       </c>
       <c r="M56" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.87549435816244625</v>
       </c>
       <c r="N56" s="11">
         <f t="shared" si="12"/>
         <v>0.86882181447580464</v>
       </c>
       <c r="O56" s="4"/>
-      <c r="P56" s="30">
+      <c r="P56" s="29">
         <v>25928</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="I59" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="J59" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K59" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L59" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="P59" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q59" s="8"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K60" s="7"/>
-      <c r="L60" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M60" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="N60" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="O60" s="18"/>
-      <c r="P60" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q60" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>0.1</v>
-      </c>
-      <c r="B61" s="11">
-        <f t="shared" ref="B61:B73" si="15">A61*$Q$5</f>
-        <v>4.0296735505064935E-2</v>
-      </c>
-      <c r="C61" s="12">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="13">
-        <v>23.784832000000002</v>
-      </c>
-      <c r="F61" s="13">
-        <v>29.746282999999998</v>
-      </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="2">
-        <v>3.52725672373683E-5</v>
-      </c>
-      <c r="I61" s="20">
-        <v>3.4288459937199994E-5</v>
-      </c>
-      <c r="J61" s="2">
-        <v>2.0764465399999998E-5</v>
-      </c>
-      <c r="K61" s="16">
-        <v>2.0531214199999999E-5</v>
-      </c>
-      <c r="L61" s="11">
-        <f>I61/H61</f>
-        <v>0.97209992418341107</v>
-      </c>
-      <c r="M61" s="11">
-        <f>J61/H61</f>
-        <v>0.58868596834090958</v>
-      </c>
-      <c r="N61" s="11">
-        <f t="shared" ref="N61:N73" si="16">K61/H61</f>
-        <v>0.58207314658539844</v>
-      </c>
-      <c r="O61" s="4"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="2"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="B62" s="9">
-        <f t="shared" si="15"/>
-        <v>0.20148367752532464</v>
-      </c>
-      <c r="C62" s="10">
-        <v>1.055E-2</v>
-      </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="6">
-        <v>10.636900000000001</v>
-      </c>
-      <c r="F62" s="6">
-        <v>13.302942</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5">
-        <v>1.76088265923015E-4</v>
-      </c>
-      <c r="I62" s="21">
-        <v>1.7111952961599997E-4</v>
-      </c>
-      <c r="J62" s="5">
-        <v>1.1061240399999999E-4</v>
-      </c>
-      <c r="K62" s="17">
-        <v>1.06846369E-4</v>
-      </c>
-      <c r="L62" s="9">
-        <f t="shared" ref="L62:L73" si="17">I62/H62</f>
-        <v>0.9717826949969095</v>
-      </c>
-      <c r="M62" s="9">
-        <f t="shared" ref="M62:M73" si="18">J62/H62</f>
-        <v>0.62816453680314643</v>
-      </c>
-      <c r="N62" s="9">
-        <f t="shared" si="16"/>
-        <v>0.60677733658137534</v>
-      </c>
-      <c r="O62" s="4"/>
-      <c r="P62" s="17"/>
-      <c r="Q62" s="5"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>1.5</v>
-      </c>
-      <c r="B63" s="11">
-        <f t="shared" si="15"/>
-        <v>0.60445103257597399</v>
-      </c>
-      <c r="C63" s="12">
-        <v>3.1649999999999998E-2</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="13">
-        <v>6.1412170000000001</v>
-      </c>
-      <c r="F63" s="13">
-        <v>7.6804569999999996</v>
-      </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="2">
-        <v>5.2684723504348998E-4</v>
-      </c>
-      <c r="I63" s="20">
-        <v>5.1184438984000003E-4</v>
-      </c>
-      <c r="J63" s="2">
-        <v>3.3546182599999996E-4</v>
-      </c>
-      <c r="K63" s="16">
-        <v>2.9865685499999995E-4</v>
-      </c>
-      <c r="L63" s="11">
-        <f t="shared" si="17"/>
-        <v>0.97152334831509268</v>
-      </c>
-      <c r="M63" s="11">
-        <f t="shared" si="18"/>
-        <v>0.63673452888541471</v>
-      </c>
-      <c r="N63" s="11">
-        <f t="shared" si="16"/>
-        <v>0.56687562377611522</v>
-      </c>
-      <c r="O63" s="4"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="2"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
-        <v>15</v>
-      </c>
-      <c r="B64" s="9">
-        <f t="shared" si="15"/>
-        <v>6.044510325759739</v>
-      </c>
-      <c r="C64" s="10">
-        <v>0.31649699999999997</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="6">
-        <v>1.9420230000000001</v>
-      </c>
-      <c r="F64" s="6">
-        <v>2.4287740000000002</v>
-      </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5">
-        <v>5.02535867346246E-3</v>
-      </c>
-      <c r="I64" s="21">
-        <v>4.88413162972E-3</v>
-      </c>
-      <c r="J64" s="5">
-        <v>3.1236285499999998E-3</v>
-      </c>
-      <c r="K64" s="17">
-        <v>2.5054505700000001E-3</v>
-      </c>
-      <c r="L64" s="9">
-        <f t="shared" si="17"/>
-        <v>0.97189712159487418</v>
-      </c>
-      <c r="M64" s="9">
-        <f t="shared" si="18"/>
-        <v>0.62157325535688124</v>
-      </c>
-      <c r="N64" s="9">
-        <f t="shared" si="16"/>
-        <v>0.4985615421304348</v>
-      </c>
-      <c r="O64" s="4"/>
-      <c r="P64" s="17"/>
-      <c r="Q64" s="5"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>30</v>
-      </c>
-      <c r="B65" s="11">
-        <f t="shared" si="15"/>
-        <v>12.089020651519478</v>
-      </c>
-      <c r="C65" s="12">
-        <v>0.63299399999999995</v>
-      </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="13">
-        <v>1.373218</v>
-      </c>
-      <c r="F65" s="13">
-        <v>1.7174020000000001</v>
-      </c>
-      <c r="G65" s="5"/>
-      <c r="H65" s="2">
-        <v>9.6096776712520909E-3</v>
-      </c>
-      <c r="I65" s="16">
-        <v>9.338383665239999E-3</v>
-      </c>
-      <c r="J65" s="2">
-        <v>6.2577857999999995E-3</v>
-      </c>
-      <c r="K65" s="16">
-        <v>5.1258882499999993E-3</v>
-      </c>
-      <c r="L65" s="11">
-        <f t="shared" si="17"/>
-        <v>0.97176866745242829</v>
-      </c>
-      <c r="M65" s="11">
-        <f t="shared" si="18"/>
-        <v>0.65119622260802035</v>
-      </c>
-      <c r="N65" s="11">
-        <f t="shared" si="16"/>
-        <v>0.5334089680587718</v>
-      </c>
-      <c r="O65" s="4"/>
-      <c r="P65" s="16"/>
-      <c r="Q65" s="2"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
-        <v>60</v>
-      </c>
-      <c r="B66" s="9">
-        <f t="shared" si="15"/>
-        <v>24.178041303038956</v>
-      </c>
-      <c r="C66" s="10">
-        <v>1.265987</v>
-      </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="6">
-        <v>0.97101199999999999</v>
-      </c>
-      <c r="F66" s="6">
-        <v>1.2143870000000001</v>
-      </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5">
-        <v>1.7956202904139199E-2</v>
-      </c>
-      <c r="I66" s="17">
-        <v>1.7408149340399998E-2</v>
-      </c>
-      <c r="J66" s="5">
-        <v>1.2780408899999998E-2</v>
-      </c>
-      <c r="K66" s="17">
-        <v>1.25560043E-2</v>
-      </c>
-      <c r="L66" s="9">
-        <f t="shared" si="17"/>
-        <v>0.96947831528385853</v>
-      </c>
-      <c r="M66" s="9">
-        <f t="shared" si="18"/>
-        <v>0.71175453787358933</v>
-      </c>
-      <c r="N66" s="9">
-        <f t="shared" si="16"/>
-        <v>0.69925720749711706</v>
-      </c>
-      <c r="O66" s="4"/>
-      <c r="P66" s="17"/>
-      <c r="Q66" s="5"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>90</v>
-      </c>
-      <c r="B67" s="11">
-        <f t="shared" si="15"/>
-        <v>36.267061954558436</v>
-      </c>
-      <c r="C67" s="12">
-        <v>1.898981</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="13">
-        <v>0.79282799999999998</v>
-      </c>
-      <c r="F67" s="13">
-        <v>0.99154299999999995</v>
-      </c>
-      <c r="G67" s="5"/>
-      <c r="H67" s="2">
-        <v>2.54716677488637E-2</v>
-      </c>
-      <c r="I67" s="16">
-        <v>2.4696861585199997E-2</v>
-      </c>
-      <c r="J67" s="2">
-        <v>1.83316504E-2</v>
-      </c>
-      <c r="K67" s="16">
-        <v>1.8560602900000001E-2</v>
-      </c>
-      <c r="L67" s="11">
-        <f t="shared" si="17"/>
-        <v>0.9695816476838951</v>
-      </c>
-      <c r="M67" s="11">
-        <f t="shared" si="18"/>
-        <v>0.71968787363040965</v>
-      </c>
-      <c r="N67" s="11">
-        <f t="shared" si="16"/>
-        <v>0.72867638990101047</v>
-      </c>
-      <c r="O67" s="4"/>
-      <c r="P67" s="16"/>
-      <c r="Q67" s="2"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
-        <v>120</v>
-      </c>
-      <c r="B68" s="9">
-        <f t="shared" si="15"/>
-        <v>48.356082606077912</v>
-      </c>
-      <c r="C68" s="10">
-        <v>2.5319750000000001</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="6">
-        <v>0.68660900000000002</v>
-      </c>
-      <c r="F68" s="6">
-        <v>0.85870100000000005</v>
-      </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5">
-        <v>3.2417642839879697E-2</v>
-      </c>
-      <c r="I68" s="17">
-        <v>3.1496843537600003E-2</v>
-      </c>
-      <c r="J68" s="5">
-        <v>2.4631987099999999E-2</v>
-      </c>
-      <c r="K68" s="17">
-        <v>2.4498665099999997E-2</v>
-      </c>
-      <c r="L68" s="9">
-        <f t="shared" si="17"/>
-        <v>0.9715957354818241</v>
-      </c>
-      <c r="M68" s="9">
-        <f t="shared" si="18"/>
-        <v>0.75983276210625961</v>
-      </c>
-      <c r="N68" s="9">
-        <f t="shared" si="16"/>
-        <v>0.75572012502593522</v>
-      </c>
-      <c r="O68" s="4"/>
-      <c r="P68" s="17"/>
-      <c r="Q68" s="5"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>150</v>
-      </c>
-      <c r="B69" s="11">
-        <f t="shared" si="15"/>
-        <v>60.445103257597395</v>
-      </c>
-      <c r="C69" s="12">
-        <v>3.1649690000000001</v>
-      </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="13">
-        <v>0.61412199999999995</v>
-      </c>
-      <c r="F69" s="13">
-        <v>0.76804600000000001</v>
-      </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="2">
-        <v>3.9055212834252402E-2</v>
-      </c>
-      <c r="I69" s="16">
-        <v>3.7975434243599997E-2</v>
-      </c>
-      <c r="J69" s="2">
-        <v>3.0206154999999998E-2</v>
-      </c>
-      <c r="K69" s="16">
-        <v>3.0258923099999998E-2</v>
-      </c>
-      <c r="L69" s="11">
-        <f t="shared" si="17"/>
-        <v>0.97235251040021442</v>
-      </c>
-      <c r="M69" s="11">
-        <f t="shared" si="18"/>
-        <v>0.77342185096245186</v>
-      </c>
-      <c r="N69" s="11">
-        <f t="shared" si="16"/>
-        <v>0.77477296637498194</v>
-      </c>
-      <c r="O69" s="4"/>
-      <c r="P69" s="16"/>
-      <c r="Q69" s="2"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
-        <v>250</v>
-      </c>
-      <c r="B70" s="9">
-        <f t="shared" si="15"/>
-        <v>100.74183876266233</v>
-      </c>
-      <c r="C70" s="10">
-        <v>5.2749480000000002</v>
-      </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="6">
-        <v>0.47569699999999998</v>
-      </c>
-      <c r="F70" s="6">
-        <v>0.59492599999999995</v>
-      </c>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5">
-        <v>5.8983323870902299E-2</v>
-      </c>
-      <c r="I70" s="17">
-        <v>5.7744756325199986E-2</v>
-      </c>
-      <c r="J70" s="5">
-        <v>4.8230853299999994E-2</v>
-      </c>
-      <c r="K70" s="17">
-        <v>4.7235667799999992E-2</v>
-      </c>
-      <c r="L70" s="9">
-        <f t="shared" si="17"/>
-        <v>0.97900139455665158</v>
-      </c>
-      <c r="M70" s="9">
-        <f t="shared" si="18"/>
-        <v>0.81770321058141104</v>
-      </c>
-      <c r="N70" s="9">
-        <f t="shared" si="16"/>
-        <v>0.80083089083594916</v>
-      </c>
-      <c r="O70" s="4"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="5"/>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>500</v>
-      </c>
-      <c r="B71" s="11">
-        <f t="shared" si="15"/>
-        <v>201.48367752532465</v>
-      </c>
-      <c r="C71" s="12">
-        <v>10.549896</v>
-      </c>
-      <c r="D71" s="4"/>
-      <c r="E71" s="13">
-        <v>0.336368</v>
-      </c>
-      <c r="F71" s="13">
-        <v>0.42067599999999999</v>
-      </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="2">
-        <v>0.103595084893309</v>
-      </c>
-      <c r="I71" s="16">
-        <v>0.10128474657560001</v>
-      </c>
-      <c r="J71" s="2">
-        <v>8.8566302999999999E-2</v>
-      </c>
-      <c r="K71" s="16">
-        <v>8.9152545999999999E-2</v>
-      </c>
-      <c r="L71" s="11">
-        <f t="shared" si="17"/>
-        <v>0.97769837902938761</v>
-      </c>
-      <c r="M71" s="11">
-        <f t="shared" si="18"/>
-        <v>0.85492765502545887</v>
-      </c>
-      <c r="N71" s="11">
-        <f t="shared" si="16"/>
-        <v>0.86058663972153548</v>
-      </c>
-      <c r="O71" s="4"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="2"/>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
-        <v>750</v>
-      </c>
-      <c r="B72" s="9">
-        <f t="shared" si="15"/>
-        <v>302.22551628798698</v>
-      </c>
-      <c r="C72" s="10">
-        <v>15.824844000000001</v>
-      </c>
-      <c r="D72" s="4"/>
-      <c r="E72" s="6">
-        <v>0.274644</v>
-      </c>
-      <c r="F72" s="6">
-        <v>0.34348000000000001</v>
-      </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5">
-        <v>0.14519436153500101</v>
-      </c>
-      <c r="I72" s="17">
-        <v>0.14184209068399997</v>
-      </c>
-      <c r="J72" s="5">
-        <v>0.12434955399999999</v>
-      </c>
-      <c r="K72" s="17">
-        <v>0.12664842399999998</v>
-      </c>
-      <c r="L72" s="9">
-        <f t="shared" si="17"/>
-        <v>0.9769118386171427</v>
-      </c>
-      <c r="M72" s="9">
-        <f t="shared" si="18"/>
-        <v>0.85643514448750746</v>
-      </c>
-      <c r="N72" s="9">
-        <f t="shared" si="16"/>
-        <v>0.87226819733953453</v>
-      </c>
-      <c r="O72" s="4"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="5"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>1000</v>
-      </c>
-      <c r="B73" s="11">
-        <f t="shared" si="15"/>
-        <v>402.9673550506493</v>
-      </c>
-      <c r="C73" s="12">
-        <v>21.09958</v>
-      </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="13">
-        <v>0.23785000000000001</v>
-      </c>
-      <c r="F73" s="13">
-        <v>0.29746400000000001</v>
-      </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="2">
-        <v>0.185920101577397</v>
-      </c>
-      <c r="I73" s="16">
-        <v>0.18159106812</v>
-      </c>
-      <c r="J73" s="2">
-        <v>0.16219431200000001</v>
-      </c>
-      <c r="K73" s="16">
-        <v>0.16194324299999999</v>
-      </c>
-      <c r="L73" s="11">
-        <f t="shared" si="17"/>
-        <v>0.97671562450392246</v>
-      </c>
-      <c r="M73" s="11">
-        <f t="shared" si="18"/>
-        <v>0.87238717397365373</v>
-      </c>
-      <c r="N73" s="11">
-        <f t="shared" si="16"/>
-        <v>0.87103676055482548</v>
-      </c>
-      <c r="O73" s="4"/>
-      <c r="P73" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
flibe, dcll, hcpb run for prod
</commit_message>
<xml_diff>
--- a/MCNP/wedge_data_2025-12-31.xlsx
+++ b/MCNP/wedge_data_2025-12-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\MCNP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78376352-570C-4FAC-9F27-6FF993714211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837CC2BB-6C87-4036-B6B1-DA2460BFBAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FC2A7-2007-48F8-8A3D-08B47124466B}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>